<commit_message>
Atualizacao de configuracoes 19/11/2024
</commit_message>
<xml_diff>
--- a/Configuracao.xlsx
+++ b/Configuracao.xlsx
@@ -1,36 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27328"/>
   <workbookPr checkCompatibility="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Codigos\Codigo_Cluster_Primeiro_Mes\Codigo Operacional\Arq_Entrada\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\remocaovies_ECMWF_ENSExtended\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8012AB7B-1CE7-4A7C-86D9-1A7DCB733369}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B119912-EC4E-4FB5-B990-E2BAC9127036}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{49340ABD-EBBA-4697-9F32-382481CBB267}"/>
+    <workbookView xWindow="75" yWindow="2010" windowWidth="25785" windowHeight="13050" xr2:uid="{49340ABD-EBBA-4697-9F32-382481CBB267}"/>
   </bookViews>
   <sheets>
     <sheet name="Dados" sheetId="1" r:id="rId1"/>
     <sheet name="MLT" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="144525"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="295">
   <si>
     <t>Agua Vermelha</t>
   </si>
@@ -849,6 +840,72 @@
   </si>
   <si>
     <t>MLT</t>
+  </si>
+  <si>
+    <t>Suica</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PSATSUIC </t>
+  </si>
+  <si>
+    <t>UHE Jirau Inc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PSATJRI  </t>
+  </si>
+  <si>
+    <t>Montante do rio Beni</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PSATBENI </t>
+  </si>
+  <si>
+    <t>PSATEPB</t>
+  </si>
+  <si>
+    <t>PSATEGM</t>
+  </si>
+  <si>
+    <t>PSATSTOA</t>
+  </si>
+  <si>
+    <t>Nova California</t>
+  </si>
+  <si>
+    <t>PSATENC</t>
+  </si>
+  <si>
+    <t>Amaru 1</t>
+  </si>
+  <si>
+    <t>PSATAMY1</t>
+  </si>
+  <si>
+    <t>Amaru 2</t>
+  </si>
+  <si>
+    <t>PSATAMY2</t>
+  </si>
+  <si>
+    <t>Amaru 3</t>
+  </si>
+  <si>
+    <t>PSATAMY3</t>
+  </si>
+  <si>
+    <t>Amaru 4</t>
+  </si>
+  <si>
+    <t>PSATAMY4</t>
+  </si>
+  <si>
+    <t>Juruena</t>
+  </si>
+  <si>
+    <t>PSATJRN</t>
+  </si>
+  <si>
+    <t>Tapajos</t>
   </si>
 </sst>
 </file>
@@ -859,7 +916,7 @@
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -901,6 +958,12 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -962,7 +1025,7 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -990,6 +1053,10 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="12">
     <cellStyle name="Incorreto" xfId="9" xr:uid="{63396630-C546-450D-BFBC-8D3E2C322B7E}"/>
@@ -1315,28 +1382,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4A63479-60F0-4FB7-958C-17C5836453DA}">
-  <dimension ref="A1:P118"/>
+  <dimension ref="A1:P130"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T52" sqref="T52"/>
+    <sheetView tabSelected="1" topLeftCell="A108" workbookViewId="0">
+      <selection activeCell="E132" sqref="E132"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.33203125" customWidth="1"/>
-    <col min="4" max="4" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.33203125" customWidth="1"/>
+    <col min="1" max="1" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.28515625" customWidth="1"/>
+    <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.28515625" customWidth="1"/>
     <col min="10" max="10" width="11" customWidth="1"/>
-    <col min="11" max="11" width="11.33203125" customWidth="1"/>
-    <col min="12" max="12" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.33203125" customWidth="1"/>
-    <col min="14" max="14" width="15.88671875" customWidth="1"/>
-    <col min="15" max="15" width="8.33203125" customWidth="1"/>
+    <col min="11" max="11" width="11.28515625" customWidth="1"/>
+    <col min="12" max="12" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.28515625" customWidth="1"/>
+    <col min="14" max="14" width="15.85546875" customWidth="1"/>
+    <col min="15" max="15" width="8.28515625" customWidth="1"/>
     <col min="16" max="16" width="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>179</v>
       </c>
@@ -1386,7 +1453,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -1436,7 +1503,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
@@ -1486,7 +1553,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
@@ -1536,7 +1603,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
@@ -1586,7 +1653,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
@@ -1636,7 +1703,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
@@ -1686,7 +1753,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>6</v>
       </c>
@@ -1736,7 +1803,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>7</v>
       </c>
@@ -1786,7 +1853,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>8</v>
       </c>
@@ -1836,7 +1903,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>9</v>
       </c>
@@ -1886,7 +1953,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>10</v>
       </c>
@@ -1936,7 +2003,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>11</v>
       </c>
@@ -1986,7 +2053,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>12</v>
       </c>
@@ -2036,7 +2103,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>13</v>
       </c>
@@ -2086,7 +2153,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>195</v>
       </c>
@@ -2136,7 +2203,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>14</v>
       </c>
@@ -2186,7 +2253,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>15</v>
       </c>
@@ -2236,7 +2303,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>16</v>
       </c>
@@ -2286,7 +2353,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>17</v>
       </c>
@@ -2336,7 +2403,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>18</v>
       </c>
@@ -2386,7 +2453,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>19</v>
       </c>
@@ -2436,7 +2503,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>20</v>
       </c>
@@ -2486,7 +2553,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>21</v>
       </c>
@@ -2536,7 +2603,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>23</v>
       </c>
@@ -2586,7 +2653,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>24</v>
       </c>
@@ -2636,7 +2703,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>26</v>
       </c>
@@ -2686,7 +2753,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>28</v>
       </c>
@@ -2736,7 +2803,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>29</v>
       </c>
@@ -2786,7 +2853,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>30</v>
       </c>
@@ -2836,7 +2903,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>31</v>
       </c>
@@ -2886,7 +2953,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>32</v>
       </c>
@@ -2936,7 +3003,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>33</v>
       </c>
@@ -2986,7 +3053,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>34</v>
       </c>
@@ -3036,7 +3103,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>35</v>
       </c>
@@ -3086,7 +3153,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>36</v>
       </c>
@@ -3136,7 +3203,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>37</v>
       </c>
@@ -3186,7 +3253,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>38</v>
       </c>
@@ -3236,7 +3303,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>39</v>
       </c>
@@ -3286,7 +3353,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>40</v>
       </c>
@@ -3336,7 +3403,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>41</v>
       </c>
@@ -3386,7 +3453,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
         <v>42</v>
       </c>
@@ -3436,7 +3503,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
         <v>43</v>
       </c>
@@ -3486,7 +3553,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
         <v>44</v>
       </c>
@@ -3536,7 +3603,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
         <v>45</v>
       </c>
@@ -3586,7 +3653,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
         <v>46</v>
       </c>
@@ -3636,7 +3703,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
         <v>47</v>
       </c>
@@ -3686,7 +3753,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
         <v>48</v>
       </c>
@@ -3736,7 +3803,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
         <v>49</v>
       </c>
@@ -3786,7 +3853,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
         <v>50</v>
       </c>
@@ -3836,7 +3903,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
         <v>51</v>
       </c>
@@ -3886,7 +3953,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
         <v>52</v>
       </c>
@@ -3936,7 +4003,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
         <v>53</v>
       </c>
@@ -3986,7 +4053,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
         <v>54</v>
       </c>
@@ -4036,7 +4103,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
         <v>55</v>
       </c>
@@ -4086,7 +4153,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
         <v>56</v>
       </c>
@@ -4136,7 +4203,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
         <v>58</v>
       </c>
@@ -4186,7 +4253,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
         <v>60</v>
       </c>
@@ -4236,7 +4303,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
         <v>62</v>
       </c>
@@ -4286,7 +4353,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
         <v>64</v>
       </c>
@@ -4336,7 +4403,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
         <v>66</v>
       </c>
@@ -4386,7 +4453,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
         <v>68</v>
       </c>
@@ -4436,7 +4503,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
         <v>70</v>
       </c>
@@ -4486,7 +4553,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
         <v>72</v>
       </c>
@@ -4536,7 +4603,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="65" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
         <v>74</v>
       </c>
@@ -4586,7 +4653,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="66" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
         <v>76</v>
       </c>
@@ -4636,7 +4703,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
         <v>78</v>
       </c>
@@ -4686,7 +4753,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="68" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
         <v>80</v>
       </c>
@@ -4736,7 +4803,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="69" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="s">
         <v>82</v>
       </c>
@@ -4786,7 +4853,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="70" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="s">
         <v>84</v>
       </c>
@@ -4836,7 +4903,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="71" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A71" s="3" t="s">
         <v>86</v>
       </c>
@@ -4886,7 +4953,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="72" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A72" s="3" t="s">
         <v>88</v>
       </c>
@@ -4936,7 +5003,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="73" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A73" s="3" t="s">
         <v>90</v>
       </c>
@@ -4986,7 +5053,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="74" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A74" s="3" t="s">
         <v>92</v>
       </c>
@@ -5036,7 +5103,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="75" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A75" s="3" t="s">
         <v>94</v>
       </c>
@@ -5086,7 +5153,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="76" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A76" s="3" t="s">
         <v>96</v>
       </c>
@@ -5136,7 +5203,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="77" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A77" s="3" t="s">
         <v>98</v>
       </c>
@@ -5186,7 +5253,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A78" s="3" t="s">
         <v>100</v>
       </c>
@@ -5236,7 +5303,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A79" s="3" t="s">
         <v>102</v>
       </c>
@@ -5286,7 +5353,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A80" s="3" t="s">
         <v>104</v>
       </c>
@@ -5336,7 +5403,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A81" s="3" t="s">
         <v>106</v>
       </c>
@@ -5386,7 +5453,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A82" s="3" t="s">
         <v>108</v>
       </c>
@@ -5436,7 +5503,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A83" s="3" t="s">
         <v>110</v>
       </c>
@@ -5486,7 +5553,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A84" s="3" t="s">
         <v>112</v>
       </c>
@@ -5536,7 +5603,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A85" s="3" t="s">
         <v>114</v>
       </c>
@@ -5586,7 +5653,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A86" s="3" t="s">
         <v>116</v>
       </c>
@@ -5636,7 +5703,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="87" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A87" s="3" t="s">
         <v>118</v>
       </c>
@@ -5686,7 +5753,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="88" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A88" s="3" t="s">
         <v>120</v>
       </c>
@@ -5736,7 +5803,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="89" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A89" s="3" t="s">
         <v>122</v>
       </c>
@@ -5786,7 +5853,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A90" s="3" t="s">
         <v>196</v>
       </c>
@@ -5836,7 +5903,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A91" s="3" t="s">
         <v>125</v>
       </c>
@@ -5886,7 +5953,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A92" s="3" t="s">
         <v>127</v>
       </c>
@@ -5936,7 +6003,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="93" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A93" s="3" t="s">
         <v>129</v>
       </c>
@@ -5986,7 +6053,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="94" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A94" s="3" t="s">
         <v>131</v>
       </c>
@@ -6036,7 +6103,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="95" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A95" s="3" t="s">
         <v>133</v>
       </c>
@@ -6086,7 +6153,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="96" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A96" s="3" t="s">
         <v>135</v>
       </c>
@@ -6136,7 +6203,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="97" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A97" s="3" t="s">
         <v>137</v>
       </c>
@@ -6186,7 +6253,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="98" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A98" s="3" t="s">
         <v>139</v>
       </c>
@@ -6236,7 +6303,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A99" s="3" t="s">
         <v>141</v>
       </c>
@@ -6286,7 +6353,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A100" s="3" t="s">
         <v>143</v>
       </c>
@@ -6336,7 +6403,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A101" s="3" t="s">
         <v>145</v>
       </c>
@@ -6386,7 +6453,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A102" s="3" t="s">
         <v>147</v>
       </c>
@@ -6436,7 +6503,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="103" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A103" s="3" t="s">
         <v>197</v>
       </c>
@@ -6486,7 +6553,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="104" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A104" s="3" t="s">
         <v>150</v>
       </c>
@@ -6536,7 +6603,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A105" s="3" t="s">
         <v>152</v>
       </c>
@@ -6586,7 +6653,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="106" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A106" s="3" t="s">
         <v>154</v>
       </c>
@@ -6636,7 +6703,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="107" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A107" s="3" t="s">
         <v>156</v>
       </c>
@@ -6686,7 +6753,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="108" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A108" s="3" t="s">
         <v>158</v>
       </c>
@@ -6736,7 +6803,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="109" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A109" s="3" t="s">
         <v>160</v>
       </c>
@@ -6786,7 +6853,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="110" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A110" s="3" t="s">
         <v>162</v>
       </c>
@@ -6836,7 +6903,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="111" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A111" s="3" t="s">
         <v>4</v>
       </c>
@@ -6886,7 +6953,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="112" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A112" s="3" t="s">
         <v>165</v>
       </c>
@@ -6936,7 +7003,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="113" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A113" s="3" t="s">
         <v>167</v>
       </c>
@@ -6986,7 +7053,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="114" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A114" s="3" t="s">
         <v>169</v>
       </c>
@@ -7036,7 +7103,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="115" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A115" s="3" t="s">
         <v>171</v>
       </c>
@@ -7086,7 +7153,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="116" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A116" s="3" t="s">
         <v>173</v>
       </c>
@@ -7136,7 +7203,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="117" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A117" s="3" t="s">
         <v>175</v>
       </c>
@@ -7186,7 +7253,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="118" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A118" s="3" t="s">
         <v>177</v>
       </c>
@@ -7234,6 +7301,210 @@
       </c>
       <c r="P118">
         <v>1</v>
+      </c>
+    </row>
+    <row r="119" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A119" s="3" t="s">
+        <v>273</v>
+      </c>
+      <c r="B119">
+        <v>-20.079999999999998</v>
+      </c>
+      <c r="C119">
+        <v>-40.58</v>
+      </c>
+      <c r="D119" t="s">
+        <v>274</v>
+      </c>
+      <c r="L119" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="120" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>275</v>
+      </c>
+      <c r="B120" s="13">
+        <v>-9.3000000000000007</v>
+      </c>
+      <c r="C120" s="13">
+        <v>-64.7</v>
+      </c>
+      <c r="D120" s="14" t="s">
+        <v>276</v>
+      </c>
+      <c r="L120" s="14" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="121" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>277</v>
+      </c>
+      <c r="B121" s="13">
+        <v>-14.59</v>
+      </c>
+      <c r="C121" s="13">
+        <v>-67.53</v>
+      </c>
+      <c r="D121" s="14" t="s">
+        <v>278</v>
+      </c>
+      <c r="L121" s="14" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="122" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
+        <v>108</v>
+      </c>
+      <c r="B122" s="5">
+        <v>-12.42</v>
+      </c>
+      <c r="C122" s="5">
+        <v>-64.42</v>
+      </c>
+      <c r="D122" t="s">
+        <v>279</v>
+      </c>
+      <c r="L122" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="123" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
+        <v>102</v>
+      </c>
+      <c r="B123" s="5">
+        <v>-10.79</v>
+      </c>
+      <c r="C123" s="5">
+        <v>-64.349999999999994</v>
+      </c>
+      <c r="D123" t="s">
+        <v>280</v>
+      </c>
+      <c r="L123" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="124" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
+        <v>114</v>
+      </c>
+      <c r="B124" s="5">
+        <v>-8.7899999999999991</v>
+      </c>
+      <c r="C124" s="5">
+        <v>-63.95</v>
+      </c>
+      <c r="D124" t="s">
+        <v>281</v>
+      </c>
+      <c r="L124" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="125" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
+        <v>282</v>
+      </c>
+      <c r="B125" s="5">
+        <v>-9.9</v>
+      </c>
+      <c r="C125" s="5">
+        <v>-66.62</v>
+      </c>
+      <c r="D125" t="s">
+        <v>283</v>
+      </c>
+      <c r="L125" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="126" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
+        <v>284</v>
+      </c>
+      <c r="B126" s="13">
+        <v>-11.71</v>
+      </c>
+      <c r="C126" s="13">
+        <v>-70.63</v>
+      </c>
+      <c r="D126" s="14" t="s">
+        <v>285</v>
+      </c>
+      <c r="L126" s="14" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="127" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
+        <v>286</v>
+      </c>
+      <c r="B127" s="13">
+        <v>-12.37</v>
+      </c>
+      <c r="C127" s="13">
+        <v>-71.17</v>
+      </c>
+      <c r="D127" s="14" t="s">
+        <v>287</v>
+      </c>
+      <c r="L127" s="14" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="128" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
+        <v>288</v>
+      </c>
+      <c r="B128" s="7">
+        <v>-13.75</v>
+      </c>
+      <c r="C128" s="7">
+        <v>-70.180000000000007</v>
+      </c>
+      <c r="D128" t="s">
+        <v>289</v>
+      </c>
+      <c r="L128" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="129" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
+        <v>290</v>
+      </c>
+      <c r="B129" s="5">
+        <v>-13.45</v>
+      </c>
+      <c r="C129" s="5">
+        <v>-69.47</v>
+      </c>
+      <c r="D129" t="s">
+        <v>291</v>
+      </c>
+      <c r="L129" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="130" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
+        <v>292</v>
+      </c>
+      <c r="B130" s="5">
+        <v>-13.37</v>
+      </c>
+      <c r="C130" s="5">
+        <v>-59.01</v>
+      </c>
+      <c r="D130" t="s">
+        <v>293</v>
+      </c>
+      <c r="L130" t="s">
+        <v>294</v>
       </c>
     </row>
   </sheetData>
@@ -7250,15 +7521,15 @@
       <selection activeCell="A2" sqref="A2:B26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.44140625" customWidth="1"/>
-    <col min="9" max="9" width="14.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.42578125" customWidth="1"/>
+    <col min="9" max="9" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>193</v>
       </c>
@@ -7266,7 +7537,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>252</v>
       </c>
@@ -7277,7 +7548,7 @@
       <c r="J2" s="10"/>
       <c r="K2" s="10"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>253</v>
       </c>
@@ -7288,7 +7559,7 @@
       <c r="J3" s="10"/>
       <c r="K3" s="10"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>254</v>
       </c>
@@ -7299,7 +7570,7 @@
       <c r="J4" s="10"/>
       <c r="K4" s="10"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>255</v>
       </c>
@@ -7310,7 +7581,7 @@
       <c r="J5" s="10"/>
       <c r="K5" s="10"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>256</v>
       </c>
@@ -7321,7 +7592,7 @@
       <c r="D6" s="10"/>
       <c r="K6" s="10"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>39</v>
       </c>
@@ -7330,7 +7601,7 @@
       </c>
       <c r="C7" s="10"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>257</v>
       </c>
@@ -7339,7 +7610,7 @@
       </c>
       <c r="C8" s="10"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>258</v>
       </c>
@@ -7348,7 +7619,7 @@
       </c>
       <c r="C9" s="10"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
         <v>259</v>
       </c>
@@ -7357,7 +7628,7 @@
       </c>
       <c r="C10" s="10"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
         <v>260</v>
       </c>
@@ -7366,7 +7637,7 @@
       </c>
       <c r="C11" s="10"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
         <v>261</v>
       </c>
@@ -7375,7 +7646,7 @@
       </c>
       <c r="C12" s="10"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
         <v>262</v>
       </c>
@@ -7384,7 +7655,7 @@
       </c>
       <c r="C13" s="10"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
         <v>263</v>
       </c>
@@ -7393,7 +7664,7 @@
       </c>
       <c r="C14" s="10"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
         <v>264</v>
       </c>
@@ -7402,7 +7673,7 @@
       </c>
       <c r="C15" s="10"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
         <v>265</v>
       </c>
@@ -7411,7 +7682,7 @@
       </c>
       <c r="C16" s="10"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
         <v>266</v>
       </c>
@@ -7420,7 +7691,7 @@
       </c>
       <c r="C17" s="10"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
         <v>267</v>
       </c>
@@ -7429,7 +7700,7 @@
       </c>
       <c r="C18" s="10"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
         <v>268</v>
       </c>
@@ -7438,7 +7709,7 @@
       </c>
       <c r="C19" s="10"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
         <v>269</v>
       </c>
@@ -7447,7 +7718,7 @@
       </c>
       <c r="C20" s="10"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
         <v>249</v>
       </c>
@@ -7456,7 +7727,7 @@
       </c>
       <c r="C21" s="10"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
         <v>7</v>
       </c>
@@ -7465,7 +7736,7 @@
       </c>
       <c r="C22" s="10"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
         <v>270</v>
       </c>
@@ -7474,7 +7745,7 @@
       </c>
       <c r="C23" s="10"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
         <v>250</v>
       </c>
@@ -7483,7 +7754,7 @@
       </c>
       <c r="C24" s="10"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
         <v>271</v>
       </c>
@@ -7492,7 +7763,7 @@
       </c>
       <c r="C25" s="10"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
         <v>251</v>
       </c>

</xml_diff>

<commit_message>
Atualizacao de configuracoes 06/12/2024 (+ PSATAPI)
</commit_message>
<xml_diff>
--- a/Configuracao.xlsx
+++ b/Configuracao.xlsx
@@ -1,27 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27328"/>
-  <workbookPr checkCompatibility="1" defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\remocaovies_ECMWF_ENSExtended\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\_serviceprh\Desktop\Ensemble\Primeiro_Mes\Codigo_Cluster_Primeiro_Mes\Codigo_Operacional\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B119912-EC4E-4FB5-B990-E2BAC9127036}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76702EF9-28B5-4C31-A03A-CC0CEAF05E93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="75" yWindow="2010" windowWidth="25785" windowHeight="13050" xr2:uid="{49340ABD-EBBA-4697-9F32-382481CBB267}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{49340ABD-EBBA-4697-9F32-382481CBB267}"/>
   </bookViews>
   <sheets>
     <sheet name="Dados" sheetId="1" r:id="rId1"/>
     <sheet name="MLT" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="191028"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="295">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="301">
   <si>
     <t>Agua Vermelha</t>
   </si>
@@ -845,67 +858,85 @@
     <t>Suica</t>
   </si>
   <si>
-    <t xml:space="preserve">PSATSUIC </t>
+    <t>PSATSUIC</t>
+  </si>
+  <si>
+    <t>Santa Maria Vitoria</t>
+  </si>
+  <si>
+    <t>Amaru Mayu 1</t>
+  </si>
+  <si>
+    <t>PSATAMY1</t>
+  </si>
+  <si>
+    <t>Amaru Mayu 2</t>
+  </si>
+  <si>
+    <t>PSATAMY2</t>
+  </si>
+  <si>
+    <t>Amaru Mayu 3</t>
+  </si>
+  <si>
+    <t>PSATAMY3</t>
+  </si>
+  <si>
+    <t>Amaru Mayu 4</t>
+  </si>
+  <si>
+    <t>PSATAMY4</t>
   </si>
   <si>
     <t>UHE Jirau Inc</t>
   </si>
   <si>
-    <t xml:space="preserve">PSATJRI  </t>
+    <t>PSATJRI</t>
   </si>
   <si>
     <t>Montante do rio Beni</t>
   </si>
   <si>
-    <t xml:space="preserve">PSATBENI </t>
+    <t>PSATBENI</t>
+  </si>
+  <si>
+    <t>Nova California</t>
+  </si>
+  <si>
+    <t>PSATENC</t>
+  </si>
+  <si>
+    <t>Estacao Guajara-Mirim</t>
+  </si>
+  <si>
+    <t>PSATEGM</t>
+  </si>
+  <si>
+    <t>Estacao Principe da Beira</t>
   </si>
   <si>
     <t>PSATEPB</t>
   </si>
   <si>
-    <t>PSATEGM</t>
+    <t>UHE Santo Antonio</t>
   </si>
   <si>
     <t>PSATSTOA</t>
   </si>
   <si>
-    <t>Nova California</t>
-  </si>
-  <si>
-    <t>PSATENC</t>
-  </si>
-  <si>
-    <t>Amaru 1</t>
-  </si>
-  <si>
-    <t>PSATAMY1</t>
-  </si>
-  <si>
-    <t>Amaru 2</t>
-  </si>
-  <si>
-    <t>PSATAMY2</t>
-  </si>
-  <si>
-    <t>Amaru 3</t>
-  </si>
-  <si>
-    <t>PSATAMY3</t>
-  </si>
-  <si>
-    <t>Amaru 4</t>
-  </si>
-  <si>
-    <t>PSATAMY4</t>
-  </si>
-  <si>
     <t>Juruena</t>
   </si>
   <si>
+    <t>Salto Apiacas</t>
+  </si>
+  <si>
     <t>PSATJRN</t>
   </si>
   <si>
-    <t>Tapajos</t>
+    <t>PSATAPI</t>
+  </si>
+  <si>
+    <t>Apiacas</t>
   </si>
 </sst>
 </file>
@@ -916,7 +947,7 @@
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -958,12 +989,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1025,7 +1050,7 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1053,10 +1078,18 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="12">
     <cellStyle name="Incorreto" xfId="9" xr:uid="{63396630-C546-450D-BFBC-8D3E2C322B7E}"/>
@@ -1382,28 +1415,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4A63479-60F0-4FB7-958C-17C5836453DA}">
-  <dimension ref="A1:P130"/>
+  <dimension ref="A1:U140"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A108" workbookViewId="0">
-      <selection activeCell="E132" sqref="E132"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B107" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="M131" sqref="M131"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="22.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.28515625" customWidth="1"/>
-    <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.28515625" customWidth="1"/>
+    <col min="1" max="1" width="22.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.26953125" customWidth="1"/>
+    <col min="4" max="4" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.26953125" customWidth="1"/>
     <col min="10" max="10" width="11" customWidth="1"/>
-    <col min="11" max="11" width="11.28515625" customWidth="1"/>
-    <col min="12" max="12" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.28515625" customWidth="1"/>
-    <col min="14" max="14" width="15.85546875" customWidth="1"/>
-    <col min="15" max="15" width="8.28515625" customWidth="1"/>
+    <col min="11" max="11" width="11.26953125" customWidth="1"/>
+    <col min="12" max="12" width="13.26953125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.26953125" customWidth="1"/>
+    <col min="14" max="14" width="15.81640625" customWidth="1"/>
+    <col min="15" max="15" width="8.26953125" customWidth="1"/>
     <col min="16" max="16" width="8" customWidth="1"/>
+    <col min="19" max="19" width="9.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" ht="26" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>179</v>
       </c>
@@ -1453,7 +1490,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -1503,7 +1540,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
@@ -1553,7 +1590,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
@@ -1603,7 +1640,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
@@ -1653,7 +1690,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
@@ -1703,7 +1740,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
@@ -1753,7 +1790,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>6</v>
       </c>
@@ -1803,7 +1840,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>7</v>
       </c>
@@ -1853,7 +1890,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>8</v>
       </c>
@@ -1903,7 +1940,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
         <v>9</v>
       </c>
@@ -1953,7 +1990,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
         <v>10</v>
       </c>
@@ -2003,7 +2040,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
         <v>11</v>
       </c>
@@ -2053,7 +2090,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
         <v>12</v>
       </c>
@@ -2103,7 +2140,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
         <v>13</v>
       </c>
@@ -2153,7 +2190,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
         <v>195</v>
       </c>
@@ -2203,7 +2240,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
         <v>14</v>
       </c>
@@ -2253,7 +2290,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
         <v>15</v>
       </c>
@@ -2303,7 +2340,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
         <v>16</v>
       </c>
@@ -2353,7 +2390,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A20" s="3" t="s">
         <v>17</v>
       </c>
@@ -2403,7 +2440,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A21" s="3" t="s">
         <v>18</v>
       </c>
@@ -2453,7 +2490,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A22" s="3" t="s">
         <v>19</v>
       </c>
@@ -2503,7 +2540,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A23" s="3" t="s">
         <v>20</v>
       </c>
@@ -2553,7 +2590,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A24" s="3" t="s">
         <v>21</v>
       </c>
@@ -2603,7 +2640,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A25" s="3" t="s">
         <v>23</v>
       </c>
@@ -2653,7 +2690,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A26" s="3" t="s">
         <v>24</v>
       </c>
@@ -2703,7 +2740,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A27" s="3" t="s">
         <v>26</v>
       </c>
@@ -2753,7 +2790,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A28" s="3" t="s">
         <v>28</v>
       </c>
@@ -2803,7 +2840,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A29" s="3" t="s">
         <v>29</v>
       </c>
@@ -2853,7 +2890,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A30" s="3" t="s">
         <v>30</v>
       </c>
@@ -2903,7 +2940,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A31" s="3" t="s">
         <v>31</v>
       </c>
@@ -2953,7 +2990,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A32" s="3" t="s">
         <v>32</v>
       </c>
@@ -3003,7 +3040,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A33" s="3" t="s">
         <v>33</v>
       </c>
@@ -3053,7 +3090,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A34" s="3" t="s">
         <v>34</v>
       </c>
@@ -3103,7 +3140,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A35" s="3" t="s">
         <v>35</v>
       </c>
@@ -3153,7 +3190,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A36" s="3" t="s">
         <v>36</v>
       </c>
@@ -3203,7 +3240,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A37" s="3" t="s">
         <v>37</v>
       </c>
@@ -3253,7 +3290,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A38" s="3" t="s">
         <v>38</v>
       </c>
@@ -3303,7 +3340,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A39" s="3" t="s">
         <v>39</v>
       </c>
@@ -3353,7 +3390,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A40" s="3" t="s">
         <v>40</v>
       </c>
@@ -3403,7 +3440,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A41" s="3" t="s">
         <v>41</v>
       </c>
@@ -3453,7 +3490,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A42" s="3" t="s">
         <v>42</v>
       </c>
@@ -3503,7 +3540,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A43" s="3" t="s">
         <v>43</v>
       </c>
@@ -3553,7 +3590,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A44" s="3" t="s">
         <v>44</v>
       </c>
@@ -3603,7 +3640,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A45" s="3" t="s">
         <v>45</v>
       </c>
@@ -3653,7 +3690,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A46" s="3" t="s">
         <v>46</v>
       </c>
@@ -3703,7 +3740,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A47" s="3" t="s">
         <v>47</v>
       </c>
@@ -3753,7 +3790,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A48" s="3" t="s">
         <v>48</v>
       </c>
@@ -3803,7 +3840,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A49" s="3" t="s">
         <v>49</v>
       </c>
@@ -3853,7 +3890,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A50" s="3" t="s">
         <v>50</v>
       </c>
@@ -3903,7 +3940,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A51" s="3" t="s">
         <v>51</v>
       </c>
@@ -3953,7 +3990,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A52" s="3" t="s">
         <v>52</v>
       </c>
@@ -4003,7 +4040,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A53" s="3" t="s">
         <v>53</v>
       </c>
@@ -4053,7 +4090,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A54" s="3" t="s">
         <v>54</v>
       </c>
@@ -4103,7 +4140,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A55" s="3" t="s">
         <v>55</v>
       </c>
@@ -4153,7 +4190,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A56" s="3" t="s">
         <v>56</v>
       </c>
@@ -4203,7 +4240,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A57" s="3" t="s">
         <v>58</v>
       </c>
@@ -4253,7 +4290,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A58" s="3" t="s">
         <v>60</v>
       </c>
@@ -4303,7 +4340,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A59" s="3" t="s">
         <v>62</v>
       </c>
@@ -4353,7 +4390,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A60" s="3" t="s">
         <v>64</v>
       </c>
@@ -4403,7 +4440,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A61" s="3" t="s">
         <v>66</v>
       </c>
@@ -4453,7 +4490,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A62" s="3" t="s">
         <v>68</v>
       </c>
@@ -4503,7 +4540,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A63" s="3" t="s">
         <v>70</v>
       </c>
@@ -4553,7 +4590,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A64" s="3" t="s">
         <v>72</v>
       </c>
@@ -4603,7 +4640,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="65" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A65" s="3" t="s">
         <v>74</v>
       </c>
@@ -4653,7 +4690,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="66" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A66" s="3" t="s">
         <v>76</v>
       </c>
@@ -4703,7 +4740,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A67" s="3" t="s">
         <v>78</v>
       </c>
@@ -4753,7 +4790,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="68" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A68" s="3" t="s">
         <v>80</v>
       </c>
@@ -4803,7 +4840,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="69" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A69" s="3" t="s">
         <v>82</v>
       </c>
@@ -4853,7 +4890,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="70" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A70" s="3" t="s">
         <v>84</v>
       </c>
@@ -4903,7 +4940,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="71" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A71" s="3" t="s">
         <v>86</v>
       </c>
@@ -4953,7 +4990,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="72" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A72" s="3" t="s">
         <v>88</v>
       </c>
@@ -5003,7 +5040,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="73" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A73" s="3" t="s">
         <v>90</v>
       </c>
@@ -5053,7 +5090,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="74" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A74" s="3" t="s">
         <v>92</v>
       </c>
@@ -5103,7 +5140,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="75" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A75" s="3" t="s">
         <v>94</v>
       </c>
@@ -5153,7 +5190,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="76" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A76" s="3" t="s">
         <v>96</v>
       </c>
@@ -5203,7 +5240,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="77" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A77" s="3" t="s">
         <v>98</v>
       </c>
@@ -5253,7 +5290,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A78" s="3" t="s">
         <v>100</v>
       </c>
@@ -5303,7 +5340,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A79" s="3" t="s">
         <v>102</v>
       </c>
@@ -5353,7 +5390,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A80" s="3" t="s">
         <v>104</v>
       </c>
@@ -5403,7 +5440,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A81" s="3" t="s">
         <v>106</v>
       </c>
@@ -5453,7 +5490,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A82" s="3" t="s">
         <v>108</v>
       </c>
@@ -5503,7 +5540,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A83" s="3" t="s">
         <v>110</v>
       </c>
@@ -5553,7 +5590,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A84" s="3" t="s">
         <v>112</v>
       </c>
@@ -5603,7 +5640,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A85" s="3" t="s">
         <v>114</v>
       </c>
@@ -5653,7 +5690,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A86" s="3" t="s">
         <v>116</v>
       </c>
@@ -5703,7 +5740,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="87" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A87" s="3" t="s">
         <v>118</v>
       </c>
@@ -5753,7 +5790,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="88" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A88" s="3" t="s">
         <v>120</v>
       </c>
@@ -5803,7 +5840,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="89" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A89" s="3" t="s">
         <v>122</v>
       </c>
@@ -5853,7 +5890,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A90" s="3" t="s">
         <v>196</v>
       </c>
@@ -5903,7 +5940,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A91" s="3" t="s">
         <v>125</v>
       </c>
@@ -5953,7 +5990,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A92" s="3" t="s">
         <v>127</v>
       </c>
@@ -6003,7 +6040,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="93" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A93" s="3" t="s">
         <v>129</v>
       </c>
@@ -6053,7 +6090,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="94" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A94" s="3" t="s">
         <v>131</v>
       </c>
@@ -6103,7 +6140,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="95" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A95" s="3" t="s">
         <v>133</v>
       </c>
@@ -6153,7 +6190,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="96" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A96" s="3" t="s">
         <v>135</v>
       </c>
@@ -6203,7 +6240,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="97" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A97" s="3" t="s">
         <v>137</v>
       </c>
@@ -6253,7 +6290,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="98" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A98" s="3" t="s">
         <v>139</v>
       </c>
@@ -6303,7 +6340,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A99" s="3" t="s">
         <v>141</v>
       </c>
@@ -6353,7 +6390,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A100" s="3" t="s">
         <v>143</v>
       </c>
@@ -6403,7 +6440,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A101" s="3" t="s">
         <v>145</v>
       </c>
@@ -6453,7 +6490,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A102" s="3" t="s">
         <v>147</v>
       </c>
@@ -6503,7 +6540,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="103" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A103" s="3" t="s">
         <v>197</v>
       </c>
@@ -6553,7 +6590,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="104" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A104" s="3" t="s">
         <v>150</v>
       </c>
@@ -6603,7 +6640,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A105" s="3" t="s">
         <v>152</v>
       </c>
@@ -6653,7 +6690,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="106" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A106" s="3" t="s">
         <v>154</v>
       </c>
@@ -6703,7 +6740,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="107" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A107" s="3" t="s">
         <v>156</v>
       </c>
@@ -6753,7 +6790,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="108" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A108" s="3" t="s">
         <v>158</v>
       </c>
@@ -6803,7 +6840,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="109" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A109" s="3" t="s">
         <v>160</v>
       </c>
@@ -6853,7 +6890,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="110" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A110" s="3" t="s">
         <v>162</v>
       </c>
@@ -6903,7 +6940,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="111" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A111" s="3" t="s">
         <v>4</v>
       </c>
@@ -6953,7 +6990,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="112" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A112" s="3" t="s">
         <v>165</v>
       </c>
@@ -7003,7 +7040,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="113" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A113" s="3" t="s">
         <v>167</v>
       </c>
@@ -7053,7 +7090,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="114" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A114" s="3" t="s">
         <v>169</v>
       </c>
@@ -7103,7 +7140,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="115" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A115" s="3" t="s">
         <v>171</v>
       </c>
@@ -7153,7 +7190,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="116" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A116" s="3" t="s">
         <v>173</v>
       </c>
@@ -7203,7 +7240,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="117" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A117" s="3" t="s">
         <v>175</v>
       </c>
@@ -7253,7 +7290,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="118" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A118" s="3" t="s">
         <v>177</v>
       </c>
@@ -7303,209 +7340,685 @@
         <v>1</v>
       </c>
     </row>
-    <row r="119" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A119" s="3" t="s">
         <v>273</v>
       </c>
-      <c r="B119">
+      <c r="B119" s="5">
         <v>-20.079999999999998</v>
       </c>
-      <c r="C119">
+      <c r="C119" s="5">
         <v>-40.58</v>
       </c>
-      <c r="D119" t="s">
+      <c r="D119" s="3" t="s">
         <v>274</v>
       </c>
+      <c r="E119" s="7">
+        <v>33</v>
+      </c>
+      <c r="F119" s="7">
+        <v>197</v>
+      </c>
+      <c r="G119" s="7">
+        <v>82</v>
+      </c>
+      <c r="H119" s="7">
+        <v>59</v>
+      </c>
+      <c r="I119" s="7">
+        <v>44</v>
+      </c>
+      <c r="J119" s="7">
+        <v>63</v>
+      </c>
+      <c r="K119" s="7">
+        <v>197</v>
+      </c>
       <c r="L119" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="120" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A120" t="s">
         <v>275</v>
       </c>
-      <c r="B120" s="13">
-        <v>-9.3000000000000007</v>
-      </c>
-      <c r="C120" s="13">
-        <v>-64.7</v>
-      </c>
-      <c r="D120" s="14" t="s">
+      <c r="M119" s="13">
+        <v>0.39</v>
+      </c>
+      <c r="N119" s="12">
+        <v>2.1132</v>
+      </c>
+      <c r="O119" s="14">
+        <v>895</v>
+      </c>
+      <c r="P119" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="120" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A120" s="3" t="s">
         <v>276</v>
       </c>
-      <c r="L120" s="14" t="s">
+      <c r="B120" s="4">
+        <v>-11.71</v>
+      </c>
+      <c r="C120" s="4">
+        <v>-70.63</v>
+      </c>
+      <c r="D120" s="3" t="s">
+        <v>277</v>
+      </c>
+      <c r="E120" s="8">
+        <v>34</v>
+      </c>
+      <c r="F120" s="8">
+        <v>158</v>
+      </c>
+      <c r="G120" s="8">
+        <v>170</v>
+      </c>
+      <c r="H120" s="8">
+        <v>99</v>
+      </c>
+      <c r="I120" s="8">
+        <v>62</v>
+      </c>
+      <c r="J120" s="8">
+        <v>80</v>
+      </c>
+      <c r="K120" s="8">
+        <v>133</v>
+      </c>
+      <c r="L120" t="s">
         <v>261</v>
       </c>
-    </row>
-    <row r="121" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A121" t="s">
-        <v>277</v>
-      </c>
-      <c r="B121" s="13">
-        <v>-14.59</v>
-      </c>
-      <c r="C121" s="13">
-        <v>-67.53</v>
-      </c>
-      <c r="D121" s="14" t="s">
+      <c r="M120" s="15">
+        <v>0.156</v>
+      </c>
+      <c r="N120" s="12">
+        <v>0</v>
+      </c>
+      <c r="O120" s="10">
+        <v>19003</v>
+      </c>
+      <c r="P120">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="121" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A121" s="3" t="s">
         <v>278</v>
       </c>
-      <c r="L121" s="14" t="s">
+      <c r="B121" s="4">
+        <v>-12.37</v>
+      </c>
+      <c r="C121" s="4">
+        <v>-71.17</v>
+      </c>
+      <c r="D121" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="E121" s="8">
+        <v>38</v>
+      </c>
+      <c r="F121" s="8">
+        <v>201</v>
+      </c>
+      <c r="G121" s="8">
+        <v>195</v>
+      </c>
+      <c r="H121" s="8">
+        <v>125</v>
+      </c>
+      <c r="I121" s="8">
+        <v>85</v>
+      </c>
+      <c r="J121" s="8">
+        <v>98</v>
+      </c>
+      <c r="K121" s="8">
+        <v>160</v>
+      </c>
+      <c r="L121" t="s">
         <v>261</v>
       </c>
-    </row>
-    <row r="122" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A122" t="s">
-        <v>108</v>
-      </c>
-      <c r="B122" s="5">
-        <v>-12.42</v>
-      </c>
-      <c r="C122" s="5">
-        <v>-64.42</v>
-      </c>
-      <c r="D122" t="s">
-        <v>279</v>
+      <c r="M121" s="15">
+        <v>0.88800000000000001</v>
+      </c>
+      <c r="N121" s="12">
+        <v>0</v>
+      </c>
+      <c r="O121" s="10">
+        <v>36539</v>
+      </c>
+      <c r="P121">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="122" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A122" s="3" t="s">
+        <v>280</v>
+      </c>
+      <c r="B122" s="4">
+        <v>-13.75</v>
+      </c>
+      <c r="C122" s="4">
+        <v>-70.180000000000007</v>
+      </c>
+      <c r="D122" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="E122" s="8">
+        <v>34</v>
+      </c>
+      <c r="F122" s="8">
+        <v>206</v>
+      </c>
+      <c r="G122" s="8">
+        <v>186</v>
+      </c>
+      <c r="H122" s="8">
+        <v>104</v>
+      </c>
+      <c r="I122" s="8">
+        <v>83</v>
+      </c>
+      <c r="J122" s="8">
+        <v>92</v>
+      </c>
+      <c r="K122" s="8">
+        <v>151</v>
       </c>
       <c r="L122" t="s">
         <v>261</v>
       </c>
-    </row>
-    <row r="123" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A123" t="s">
+      <c r="M122" s="15">
+        <v>0.88400000000000001</v>
+      </c>
+      <c r="N122" s="12">
+        <v>0</v>
+      </c>
+      <c r="O122" s="10">
+        <v>19623</v>
+      </c>
+      <c r="P122">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="123" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A123" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="B123" s="4">
+        <v>-13.45</v>
+      </c>
+      <c r="C123" s="4">
+        <v>-69.47</v>
+      </c>
+      <c r="D123" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="E123" s="8">
+        <v>45</v>
+      </c>
+      <c r="F123" s="8">
+        <v>239</v>
+      </c>
+      <c r="G123" s="8">
+        <v>215</v>
+      </c>
+      <c r="H123" s="8">
+        <v>128</v>
+      </c>
+      <c r="I123" s="8">
+        <v>132</v>
+      </c>
+      <c r="J123" s="8">
         <v>102</v>
       </c>
-      <c r="B123" s="5">
-        <v>-10.79</v>
-      </c>
-      <c r="C123" s="5">
-        <v>-64.349999999999994</v>
-      </c>
-      <c r="D123" t="s">
-        <v>280</v>
+      <c r="K123" s="8">
+        <v>169</v>
       </c>
       <c r="L123" t="s">
         <v>261</v>
       </c>
-    </row>
-    <row r="124" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A124" t="s">
-        <v>114</v>
-      </c>
-      <c r="B124" s="5">
-        <v>-8.7899999999999991</v>
-      </c>
-      <c r="C124" s="5">
-        <v>-63.95</v>
-      </c>
-      <c r="D124" t="s">
-        <v>281</v>
+      <c r="M123" s="15">
+        <v>0.61</v>
+      </c>
+      <c r="N123" s="12">
+        <v>0</v>
+      </c>
+      <c r="O123" s="10">
+        <v>15581</v>
+      </c>
+      <c r="P123">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="124" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A124" s="3" t="s">
+        <v>284</v>
+      </c>
+      <c r="B124" s="4">
+        <v>-9.3000000000000007</v>
+      </c>
+      <c r="C124" s="4">
+        <v>-64.7</v>
+      </c>
+      <c r="D124" s="3" t="s">
+        <v>285</v>
+      </c>
+      <c r="E124" s="8">
+        <v>25</v>
+      </c>
+      <c r="F124" s="8">
+        <v>149</v>
+      </c>
+      <c r="G124" s="8">
+        <v>147</v>
+      </c>
+      <c r="H124" s="8">
+        <v>79</v>
+      </c>
+      <c r="I124" s="8">
+        <v>43</v>
+      </c>
+      <c r="J124" s="8">
+        <v>63</v>
+      </c>
+      <c r="K124" s="8">
+        <v>118</v>
       </c>
       <c r="L124" t="s">
         <v>261</v>
       </c>
-    </row>
-    <row r="125" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A125" t="s">
-        <v>282</v>
-      </c>
-      <c r="B125" s="5">
-        <v>-9.9</v>
-      </c>
-      <c r="C125" s="5">
-        <v>-66.62</v>
-      </c>
-      <c r="D125" t="s">
-        <v>283</v>
+      <c r="M124" s="15">
+        <v>0.247</v>
+      </c>
+      <c r="N124" s="12">
+        <v>0</v>
+      </c>
+      <c r="O124">
+        <v>172358</v>
+      </c>
+      <c r="P124">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="125" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A125" s="3" t="s">
+        <v>286</v>
+      </c>
+      <c r="B125" s="4">
+        <v>-14.59</v>
+      </c>
+      <c r="C125" s="4">
+        <v>-67.53</v>
+      </c>
+      <c r="D125" s="3" t="s">
+        <v>287</v>
+      </c>
+      <c r="E125" s="8">
+        <v>22</v>
+      </c>
+      <c r="F125" s="8">
+        <v>123</v>
+      </c>
+      <c r="G125" s="8">
+        <v>113</v>
+      </c>
+      <c r="H125" s="8">
+        <v>53</v>
+      </c>
+      <c r="I125" s="8">
+        <v>31</v>
+      </c>
+      <c r="J125" s="8">
+        <v>60</v>
+      </c>
+      <c r="K125" s="8">
+        <v>89</v>
       </c>
       <c r="L125" t="s">
         <v>261</v>
       </c>
-    </row>
-    <row r="126" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A126" t="s">
-        <v>284</v>
-      </c>
-      <c r="B126" s="13">
-        <v>-11.71</v>
-      </c>
-      <c r="C126" s="13">
-        <v>-70.63</v>
-      </c>
-      <c r="D126" s="14" t="s">
-        <v>285</v>
-      </c>
-      <c r="L126" s="14" t="s">
+      <c r="M125" s="15">
+        <v>0.54900000000000004</v>
+      </c>
+      <c r="N125" s="12">
+        <v>0</v>
+      </c>
+      <c r="O125" s="18">
+        <v>69743.245636194202</v>
+      </c>
+      <c r="P125">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="126" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A126" s="3" t="s">
+        <v>288</v>
+      </c>
+      <c r="B126" s="4">
+        <v>-9.9</v>
+      </c>
+      <c r="C126" s="4">
+        <v>-66.62</v>
+      </c>
+      <c r="D126" s="3" t="s">
+        <v>289</v>
+      </c>
+      <c r="E126" s="8">
+        <v>30</v>
+      </c>
+      <c r="F126" s="8">
+        <v>135</v>
+      </c>
+      <c r="G126" s="8">
+        <v>146</v>
+      </c>
+      <c r="H126" s="8">
+        <v>83</v>
+      </c>
+      <c r="I126" s="8">
+        <v>35</v>
+      </c>
+      <c r="J126" s="8">
+        <v>73</v>
+      </c>
+      <c r="K126" s="8">
+        <v>124</v>
+      </c>
+      <c r="L126" t="s">
         <v>261</v>
       </c>
-    </row>
-    <row r="127" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A127" t="s">
-        <v>286</v>
-      </c>
-      <c r="B127" s="13">
-        <v>-12.37</v>
-      </c>
-      <c r="C127" s="13">
-        <v>-71.17</v>
-      </c>
-      <c r="D127" s="14" t="s">
-        <v>287</v>
-      </c>
-      <c r="L127" s="14" t="s">
+      <c r="M126" s="15">
+        <v>1.1870000000000001</v>
+      </c>
+      <c r="N126" s="12">
+        <v>0</v>
+      </c>
+      <c r="O126" s="18">
+        <v>12513.4835015523</v>
+      </c>
+      <c r="P126">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="127" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A127" s="3" t="s">
+        <v>290</v>
+      </c>
+      <c r="B127" s="4">
+        <v>-10.79</v>
+      </c>
+      <c r="C127" s="4">
+        <v>-64.349999999999994</v>
+      </c>
+      <c r="D127" s="3" t="s">
+        <v>291</v>
+      </c>
+      <c r="E127" s="6">
+        <v>25</v>
+      </c>
+      <c r="F127" s="6">
+        <v>141</v>
+      </c>
+      <c r="G127" s="6">
+        <v>124</v>
+      </c>
+      <c r="H127" s="6">
+        <v>67</v>
+      </c>
+      <c r="I127" s="6">
+        <v>46</v>
+      </c>
+      <c r="J127" s="6">
+        <v>54</v>
+      </c>
+      <c r="K127" s="6">
+        <v>104</v>
+      </c>
+      <c r="L127" t="s">
         <v>261</v>
       </c>
-    </row>
-    <row r="128" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A128" t="s">
-        <v>288</v>
-      </c>
-      <c r="B128" s="7">
-        <v>-13.75</v>
-      </c>
-      <c r="C128" s="7">
-        <v>-70.180000000000007</v>
-      </c>
-      <c r="D128" t="s">
-        <v>289</v>
+      <c r="M127" s="15">
+        <v>0.375</v>
+      </c>
+      <c r="N127" s="12">
+        <v>0</v>
+      </c>
+      <c r="O127">
+        <v>269836</v>
+      </c>
+      <c r="P127">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="128" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A128" s="3" t="s">
+        <v>292</v>
+      </c>
+      <c r="B128" s="4">
+        <v>-12.42</v>
+      </c>
+      <c r="C128" s="4">
+        <v>-64.42</v>
+      </c>
+      <c r="D128" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="E128" s="6">
+        <v>23</v>
+      </c>
+      <c r="F128" s="6">
+        <v>116</v>
+      </c>
+      <c r="G128" s="6">
+        <v>95</v>
+      </c>
+      <c r="H128" s="6">
+        <v>51</v>
+      </c>
+      <c r="I128" s="6">
+        <v>14</v>
+      </c>
+      <c r="J128" s="6">
+        <v>36</v>
+      </c>
+      <c r="K128" s="6">
+        <v>83</v>
       </c>
       <c r="L128" t="s">
         <v>261</v>
       </c>
-    </row>
-    <row r="129" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A129" t="s">
-        <v>290</v>
-      </c>
-      <c r="B129" s="5">
-        <v>-13.45</v>
-      </c>
-      <c r="C129" s="5">
-        <v>-69.47</v>
-      </c>
-      <c r="D129" t="s">
-        <v>291</v>
+      <c r="M128" s="15">
+        <v>0.13100000000000001</v>
+      </c>
+      <c r="N128" s="12">
+        <v>0</v>
+      </c>
+      <c r="O128">
+        <v>345524</v>
+      </c>
+      <c r="P128">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="129" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A129" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="B129" s="4">
+        <v>-8.7899999999999991</v>
+      </c>
+      <c r="C129" s="4">
+        <v>-63.95</v>
+      </c>
+      <c r="D129" s="3" t="s">
+        <v>295</v>
+      </c>
+      <c r="E129" s="6">
+        <v>25</v>
+      </c>
+      <c r="F129" s="6">
+        <v>138</v>
+      </c>
+      <c r="G129" s="6">
+        <v>140</v>
+      </c>
+      <c r="H129" s="6">
+        <v>76</v>
+      </c>
+      <c r="I129" s="6">
+        <v>24</v>
+      </c>
+      <c r="J129" s="6">
+        <v>67</v>
+      </c>
+      <c r="K129" s="6">
+        <v>116</v>
       </c>
       <c r="L129" t="s">
         <v>261</v>
       </c>
-    </row>
-    <row r="130" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A130" t="s">
-        <v>292</v>
-      </c>
-      <c r="B130" s="5">
+      <c r="M129" s="15">
+        <v>0.32300000000000001</v>
+      </c>
+      <c r="N129" s="12">
+        <v>0</v>
+      </c>
+      <c r="O129">
+        <v>17113</v>
+      </c>
+      <c r="P129">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="130" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A130" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="B130" s="4">
         <v>-13.37</v>
       </c>
-      <c r="C130" s="5">
+      <c r="C130" s="4">
         <v>-59.01</v>
       </c>
-      <c r="D130" t="s">
-        <v>293</v>
+      <c r="D130" s="3" t="s">
+        <v>298</v>
+      </c>
+      <c r="E130" s="7">
+        <v>26</v>
+      </c>
+      <c r="F130" s="7">
+        <v>145</v>
+      </c>
+      <c r="G130" s="7">
+        <v>129</v>
+      </c>
+      <c r="H130" s="7">
+        <v>74</v>
+      </c>
+      <c r="I130" s="7">
+        <v>19</v>
+      </c>
+      <c r="J130" s="7">
+        <v>61</v>
+      </c>
+      <c r="K130" s="7">
+        <v>104</v>
       </c>
       <c r="L130" t="s">
-        <v>294</v>
-      </c>
+        <v>296</v>
+      </c>
+      <c r="M130" s="15">
+        <v>0.57299999999999995</v>
+      </c>
+      <c r="N130" s="12">
+        <v>0</v>
+      </c>
+      <c r="O130">
+        <v>4574</v>
+      </c>
+      <c r="P130">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="131" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A131" s="3" t="s">
+        <v>297</v>
+      </c>
+      <c r="B131" s="4">
+        <v>-10.34</v>
+      </c>
+      <c r="C131" s="4">
+        <v>-56.98</v>
+      </c>
+      <c r="D131" s="3" t="s">
+        <v>299</v>
+      </c>
+      <c r="E131" s="7">
+        <v>31</v>
+      </c>
+      <c r="F131" s="7">
+        <v>175</v>
+      </c>
+      <c r="G131" s="7">
+        <v>160</v>
+      </c>
+      <c r="H131" s="7">
+        <v>91</v>
+      </c>
+      <c r="I131" s="7">
+        <v>9</v>
+      </c>
+      <c r="J131" s="7">
+        <v>68</v>
+      </c>
+      <c r="K131" s="7">
+        <v>145</v>
+      </c>
+      <c r="L131" t="s">
+        <v>300</v>
+      </c>
+      <c r="M131" s="15">
+        <v>0.434</v>
+      </c>
+      <c r="N131" s="12">
+        <v>0</v>
+      </c>
+      <c r="O131">
+        <v>7267</v>
+      </c>
+      <c r="P131">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="135" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="S135" s="17"/>
+      <c r="T135" s="17"/>
+      <c r="U135" s="18"/>
+    </row>
+    <row r="136" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="S136" s="17"/>
+      <c r="T136" s="17"/>
+      <c r="U136" s="18"/>
+    </row>
+    <row r="137" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="S137" s="17"/>
+      <c r="T137" s="17"/>
+      <c r="U137" s="18"/>
+    </row>
+    <row r="138" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="S138" s="16"/>
+      <c r="T138" s="16"/>
+      <c r="U138" s="16"/>
+    </row>
+    <row r="139" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="S139" s="16"/>
+      <c r="T139" s="16"/>
+      <c r="U139" s="16"/>
+    </row>
+    <row r="140" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="S140" s="16"/>
+      <c r="T140" s="16"/>
+      <c r="U140" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -7515,21 +8028,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77DEB068-3F58-4E33-9788-A70044A01109}">
-  <dimension ref="A1:K26"/>
+  <dimension ref="A1:K29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B26"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.42578125" customWidth="1"/>
-    <col min="9" max="9" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.26953125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.453125" customWidth="1"/>
+    <col min="9" max="9" width="14.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>193</v>
       </c>
@@ -7537,7 +8050,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" s="9" t="s">
         <v>252</v>
       </c>
@@ -7548,7 +8061,7 @@
       <c r="J2" s="10"/>
       <c r="K2" s="10"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" s="9" t="s">
         <v>253</v>
       </c>
@@ -7559,7 +8072,7 @@
       <c r="J3" s="10"/>
       <c r="K3" s="10"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" s="9" t="s">
         <v>254</v>
       </c>
@@ -7570,7 +8083,7 @@
       <c r="J4" s="10"/>
       <c r="K4" s="10"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" s="9" t="s">
         <v>255</v>
       </c>
@@ -7581,7 +8094,7 @@
       <c r="J5" s="10"/>
       <c r="K5" s="10"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" s="9" t="s">
         <v>256</v>
       </c>
@@ -7592,7 +8105,7 @@
       <c r="D6" s="10"/>
       <c r="K6" s="10"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" s="9" t="s">
         <v>39</v>
       </c>
@@ -7601,7 +8114,7 @@
       </c>
       <c r="C7" s="10"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" s="9" t="s">
         <v>257</v>
       </c>
@@ -7610,7 +8123,7 @@
       </c>
       <c r="C8" s="10"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" s="9" t="s">
         <v>258</v>
       </c>
@@ -7619,7 +8132,7 @@
       </c>
       <c r="C9" s="10"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" s="9" t="s">
         <v>259</v>
       </c>
@@ -7628,7 +8141,7 @@
       </c>
       <c r="C10" s="10"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" s="9" t="s">
         <v>260</v>
       </c>
@@ -7637,7 +8150,7 @@
       </c>
       <c r="C11" s="10"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12" s="9" t="s">
         <v>261</v>
       </c>
@@ -7646,7 +8159,7 @@
       </c>
       <c r="C12" s="10"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13" s="9" t="s">
         <v>262</v>
       </c>
@@ -7655,7 +8168,7 @@
       </c>
       <c r="C13" s="10"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A14" s="9" t="s">
         <v>263</v>
       </c>
@@ -7664,7 +8177,7 @@
       </c>
       <c r="C14" s="10"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15" s="9" t="s">
         <v>264</v>
       </c>
@@ -7673,7 +8186,7 @@
       </c>
       <c r="C15" s="10"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A16" s="9" t="s">
         <v>265</v>
       </c>
@@ -7682,7 +8195,7 @@
       </c>
       <c r="C16" s="10"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" s="9" t="s">
         <v>266</v>
       </c>
@@ -7691,7 +8204,7 @@
       </c>
       <c r="C17" s="10"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" s="9" t="s">
         <v>267</v>
       </c>
@@ -7700,7 +8213,7 @@
       </c>
       <c r="C18" s="10"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" s="9" t="s">
         <v>268</v>
       </c>
@@ -7709,7 +8222,7 @@
       </c>
       <c r="C19" s="10"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" s="9" t="s">
         <v>269</v>
       </c>
@@ -7718,7 +8231,7 @@
       </c>
       <c r="C20" s="10"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" s="9" t="s">
         <v>249</v>
       </c>
@@ -7727,7 +8240,7 @@
       </c>
       <c r="C21" s="10"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" s="9" t="s">
         <v>7</v>
       </c>
@@ -7736,7 +8249,7 @@
       </c>
       <c r="C22" s="10"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" s="9" t="s">
         <v>270</v>
       </c>
@@ -7745,7 +8258,7 @@
       </c>
       <c r="C23" s="10"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" s="9" t="s">
         <v>250</v>
       </c>
@@ -7754,7 +8267,7 @@
       </c>
       <c r="C24" s="10"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" s="9" t="s">
         <v>271</v>
       </c>
@@ -7763,7 +8276,7 @@
       </c>
       <c r="C25" s="10"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" s="9" t="s">
         <v>251</v>
       </c>
@@ -7771,6 +8284,30 @@
         <v>1132</v>
       </c>
       <c r="C26" s="10"/>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A27" s="9" t="s">
+        <v>275</v>
+      </c>
+      <c r="B27" s="11">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A28" s="9" t="s">
+        <v>296</v>
+      </c>
+      <c r="B28" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A29" s="9" t="s">
+        <v>300</v>
+      </c>
+      <c r="B29" s="11">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>

<commit_message>
Atualizacao de configuracoes 24/04/2025 (+PSATSALT): arquivo(s) de entrada exemplo(s)
</commit_message>
<xml_diff>
--- a/Configuracao.xlsx
+++ b/Configuracao.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\_serviceprh\Desktop\Ensemble\Primeiro_Mes\Codigo_Cluster_Primeiro_Mes\Codigo_Operacional\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\remocaovies_ECMWF_ENSExtended\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76702EF9-28B5-4C31-A03A-CC0CEAF05E93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFDC99D0-722C-47D4-B4AF-7350C53B87A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{49340ABD-EBBA-4697-9F32-382481CBB267}"/>
+    <workbookView xWindow="945" yWindow="2025" windowWidth="26745" windowHeight="11385" xr2:uid="{49340ABD-EBBA-4697-9F32-382481CBB267}"/>
   </bookViews>
   <sheets>
     <sheet name="Dados" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="301">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="304">
   <si>
     <t>Agua Vermelha</t>
   </si>
@@ -937,6 +937,15 @@
   </si>
   <si>
     <t>Apiacas</t>
+  </si>
+  <si>
+    <t>UHE Canastra</t>
+  </si>
+  <si>
+    <t>PSATSALT</t>
+  </si>
+  <si>
+    <t>Cai</t>
   </si>
 </sst>
 </file>
@@ -1119,9 +1128,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office 2013 - 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1159,7 +1168,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1265,7 +1274,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1407,7 +1416,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1418,29 +1427,29 @@
   <dimension ref="A1:U140"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B107" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B125" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="M131" sqref="M131"/>
+      <selection pane="bottomRight" activeCell="M132" sqref="M132"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.26953125" customWidth="1"/>
-    <col min="4" max="4" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.26953125" customWidth="1"/>
+    <col min="1" max="1" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.28515625" customWidth="1"/>
+    <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.28515625" customWidth="1"/>
     <col min="10" max="10" width="11" customWidth="1"/>
-    <col min="11" max="11" width="11.26953125" customWidth="1"/>
-    <col min="12" max="12" width="13.26953125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.26953125" customWidth="1"/>
-    <col min="14" max="14" width="15.81640625" customWidth="1"/>
-    <col min="15" max="15" width="8.26953125" customWidth="1"/>
+    <col min="11" max="11" width="11.28515625" customWidth="1"/>
+    <col min="12" max="12" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.28515625" customWidth="1"/>
+    <col min="14" max="14" width="15.85546875" customWidth="1"/>
+    <col min="15" max="15" width="8.28515625" customWidth="1"/>
     <col min="16" max="16" width="8" customWidth="1"/>
-    <col min="19" max="19" width="9.90625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="26" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>179</v>
       </c>
@@ -1490,7 +1499,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -1540,7 +1549,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
@@ -1590,7 +1599,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
@@ -1640,7 +1649,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
@@ -1690,7 +1699,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
@@ -1740,7 +1749,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
@@ -1790,7 +1799,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>6</v>
       </c>
@@ -1840,7 +1849,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>7</v>
       </c>
@@ -1890,7 +1899,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>8</v>
       </c>
@@ -1940,7 +1949,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>9</v>
       </c>
@@ -1990,7 +1999,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>10</v>
       </c>
@@ -2040,7 +2049,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>11</v>
       </c>
@@ -2090,7 +2099,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>12</v>
       </c>
@@ -2140,7 +2149,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>13</v>
       </c>
@@ -2190,7 +2199,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>195</v>
       </c>
@@ -2240,7 +2249,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>14</v>
       </c>
@@ -2290,7 +2299,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>15</v>
       </c>
@@ -2340,7 +2349,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>16</v>
       </c>
@@ -2390,7 +2399,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>17</v>
       </c>
@@ -2440,7 +2449,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>18</v>
       </c>
@@ -2490,7 +2499,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>19</v>
       </c>
@@ -2540,7 +2549,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>20</v>
       </c>
@@ -2590,7 +2599,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>21</v>
       </c>
@@ -2640,7 +2649,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>23</v>
       </c>
@@ -2690,7 +2699,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>24</v>
       </c>
@@ -2740,7 +2749,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>26</v>
       </c>
@@ -2790,7 +2799,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>28</v>
       </c>
@@ -2840,7 +2849,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>29</v>
       </c>
@@ -2890,7 +2899,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>30</v>
       </c>
@@ -2940,7 +2949,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>31</v>
       </c>
@@ -2990,7 +2999,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>32</v>
       </c>
@@ -3040,7 +3049,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>33</v>
       </c>
@@ -3090,7 +3099,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>34</v>
       </c>
@@ -3140,7 +3149,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>35</v>
       </c>
@@ -3190,7 +3199,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>36</v>
       </c>
@@ -3240,7 +3249,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>37</v>
       </c>
@@ -3290,7 +3299,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>38</v>
       </c>
@@ -3340,7 +3349,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>39</v>
       </c>
@@ -3390,7 +3399,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>40</v>
       </c>
@@ -3440,7 +3449,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>41</v>
       </c>
@@ -3490,7 +3499,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
         <v>42</v>
       </c>
@@ -3540,7 +3549,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
         <v>43</v>
       </c>
@@ -3590,7 +3599,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
         <v>44</v>
       </c>
@@ -3640,7 +3649,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
         <v>45</v>
       </c>
@@ -3690,7 +3699,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
         <v>46</v>
       </c>
@@ -3740,7 +3749,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
         <v>47</v>
       </c>
@@ -3790,7 +3799,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
         <v>48</v>
       </c>
@@ -3840,7 +3849,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
         <v>49</v>
       </c>
@@ -3890,7 +3899,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
         <v>50</v>
       </c>
@@ -3940,7 +3949,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
         <v>51</v>
       </c>
@@ -3990,7 +3999,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
         <v>52</v>
       </c>
@@ -4040,7 +4049,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
         <v>53</v>
       </c>
@@ -4090,7 +4099,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
         <v>54</v>
       </c>
@@ -4140,7 +4149,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
         <v>55</v>
       </c>
@@ -4190,7 +4199,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
         <v>56</v>
       </c>
@@ -4240,7 +4249,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
         <v>58</v>
       </c>
@@ -4290,7 +4299,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
         <v>60</v>
       </c>
@@ -4340,7 +4349,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
         <v>62</v>
       </c>
@@ -4390,7 +4399,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
         <v>64</v>
       </c>
@@ -4440,7 +4449,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
         <v>66</v>
       </c>
@@ -4490,7 +4499,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
         <v>68</v>
       </c>
@@ -4540,7 +4549,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
         <v>70</v>
       </c>
@@ -4590,7 +4599,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
         <v>72</v>
       </c>
@@ -4640,7 +4649,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="65" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
         <v>74</v>
       </c>
@@ -4690,7 +4699,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="66" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
         <v>76</v>
       </c>
@@ -4740,7 +4749,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
         <v>78</v>
       </c>
@@ -4790,7 +4799,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="68" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
         <v>80</v>
       </c>
@@ -4840,7 +4849,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="69" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="s">
         <v>82</v>
       </c>
@@ -4890,7 +4899,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="70" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="s">
         <v>84</v>
       </c>
@@ -4940,7 +4949,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="71" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A71" s="3" t="s">
         <v>86</v>
       </c>
@@ -4990,7 +4999,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="72" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A72" s="3" t="s">
         <v>88</v>
       </c>
@@ -5040,7 +5049,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="73" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A73" s="3" t="s">
         <v>90</v>
       </c>
@@ -5090,7 +5099,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="74" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A74" s="3" t="s">
         <v>92</v>
       </c>
@@ -5140,7 +5149,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="75" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A75" s="3" t="s">
         <v>94</v>
       </c>
@@ -5190,7 +5199,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="76" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A76" s="3" t="s">
         <v>96</v>
       </c>
@@ -5240,7 +5249,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="77" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A77" s="3" t="s">
         <v>98</v>
       </c>
@@ -5290,7 +5299,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A78" s="3" t="s">
         <v>100</v>
       </c>
@@ -5340,7 +5349,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A79" s="3" t="s">
         <v>102</v>
       </c>
@@ -5390,7 +5399,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A80" s="3" t="s">
         <v>104</v>
       </c>
@@ -5440,7 +5449,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A81" s="3" t="s">
         <v>106</v>
       </c>
@@ -5490,7 +5499,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A82" s="3" t="s">
         <v>108</v>
       </c>
@@ -5540,7 +5549,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A83" s="3" t="s">
         <v>110</v>
       </c>
@@ -5590,7 +5599,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A84" s="3" t="s">
         <v>112</v>
       </c>
@@ -5640,7 +5649,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A85" s="3" t="s">
         <v>114</v>
       </c>
@@ -5690,7 +5699,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A86" s="3" t="s">
         <v>116</v>
       </c>
@@ -5740,7 +5749,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="87" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A87" s="3" t="s">
         <v>118</v>
       </c>
@@ -5790,7 +5799,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="88" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A88" s="3" t="s">
         <v>120</v>
       </c>
@@ -5840,7 +5849,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="89" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A89" s="3" t="s">
         <v>122</v>
       </c>
@@ -5890,7 +5899,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A90" s="3" t="s">
         <v>196</v>
       </c>
@@ -5940,7 +5949,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A91" s="3" t="s">
         <v>125</v>
       </c>
@@ -5990,7 +5999,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A92" s="3" t="s">
         <v>127</v>
       </c>
@@ -6040,7 +6049,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="93" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A93" s="3" t="s">
         <v>129</v>
       </c>
@@ -6090,7 +6099,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="94" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A94" s="3" t="s">
         <v>131</v>
       </c>
@@ -6140,7 +6149,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="95" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A95" s="3" t="s">
         <v>133</v>
       </c>
@@ -6190,7 +6199,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="96" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A96" s="3" t="s">
         <v>135</v>
       </c>
@@ -6240,7 +6249,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="97" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A97" s="3" t="s">
         <v>137</v>
       </c>
@@ -6290,7 +6299,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="98" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A98" s="3" t="s">
         <v>139</v>
       </c>
@@ -6340,7 +6349,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A99" s="3" t="s">
         <v>141</v>
       </c>
@@ -6390,7 +6399,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A100" s="3" t="s">
         <v>143</v>
       </c>
@@ -6440,7 +6449,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A101" s="3" t="s">
         <v>145</v>
       </c>
@@ -6490,7 +6499,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A102" s="3" t="s">
         <v>147</v>
       </c>
@@ -6540,7 +6549,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="103" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A103" s="3" t="s">
         <v>197</v>
       </c>
@@ -6590,7 +6599,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="104" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A104" s="3" t="s">
         <v>150</v>
       </c>
@@ -6640,7 +6649,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A105" s="3" t="s">
         <v>152</v>
       </c>
@@ -6690,7 +6699,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="106" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A106" s="3" t="s">
         <v>154</v>
       </c>
@@ -6740,7 +6749,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="107" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A107" s="3" t="s">
         <v>156</v>
       </c>
@@ -6790,7 +6799,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="108" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A108" s="3" t="s">
         <v>158</v>
       </c>
@@ -6840,7 +6849,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="109" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A109" s="3" t="s">
         <v>160</v>
       </c>
@@ -6890,7 +6899,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="110" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A110" s="3" t="s">
         <v>162</v>
       </c>
@@ -6940,7 +6949,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="111" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A111" s="3" t="s">
         <v>4</v>
       </c>
@@ -6990,7 +6999,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="112" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A112" s="3" t="s">
         <v>165</v>
       </c>
@@ -7040,7 +7049,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="113" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A113" s="3" t="s">
         <v>167</v>
       </c>
@@ -7090,7 +7099,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="114" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A114" s="3" t="s">
         <v>169</v>
       </c>
@@ -7140,7 +7149,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="115" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A115" s="3" t="s">
         <v>171</v>
       </c>
@@ -7190,7 +7199,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="116" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A116" s="3" t="s">
         <v>173</v>
       </c>
@@ -7240,7 +7249,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="117" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A117" s="3" t="s">
         <v>175</v>
       </c>
@@ -7290,7 +7299,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="118" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A118" s="3" t="s">
         <v>177</v>
       </c>
@@ -7340,7 +7349,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="119" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A119" s="3" t="s">
         <v>273</v>
       </c>
@@ -7390,7 +7399,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="120" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A120" s="3" t="s">
         <v>276</v>
       </c>
@@ -7440,7 +7449,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="121" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A121" s="3" t="s">
         <v>278</v>
       </c>
@@ -7490,7 +7499,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="122" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A122" s="3" t="s">
         <v>280</v>
       </c>
@@ -7540,7 +7549,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="123" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A123" s="3" t="s">
         <v>282</v>
       </c>
@@ -7590,7 +7599,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="124" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A124" s="3" t="s">
         <v>284</v>
       </c>
@@ -7640,7 +7649,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="125" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A125" s="3" t="s">
         <v>286</v>
       </c>
@@ -7690,7 +7699,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="126" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A126" s="3" t="s">
         <v>288</v>
       </c>
@@ -7740,7 +7749,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="127" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A127" s="3" t="s">
         <v>290</v>
       </c>
@@ -7790,7 +7799,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="128" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A128" s="3" t="s">
         <v>292</v>
       </c>
@@ -7840,7 +7849,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="129" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A129" s="3" t="s">
         <v>294</v>
       </c>
@@ -7890,7 +7899,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="130" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A130" s="3" t="s">
         <v>296</v>
       </c>
@@ -7940,7 +7949,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="131" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A131" s="3" t="s">
         <v>297</v>
       </c>
@@ -7990,32 +7999,49 @@
         <v>1</v>
       </c>
     </row>
-    <row r="135" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A132" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="B132" s="5">
+        <v>-29.32</v>
+      </c>
+      <c r="C132" s="5">
+        <v>-50.68</v>
+      </c>
+      <c r="D132" s="3" t="s">
+        <v>302</v>
+      </c>
+      <c r="L132" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="135" spans="1:21" x14ac:dyDescent="0.25">
       <c r="S135" s="17"/>
       <c r="T135" s="17"/>
       <c r="U135" s="18"/>
     </row>
-    <row r="136" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:21" x14ac:dyDescent="0.25">
       <c r="S136" s="17"/>
       <c r="T136" s="17"/>
       <c r="U136" s="18"/>
     </row>
-    <row r="137" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:21" x14ac:dyDescent="0.25">
       <c r="S137" s="17"/>
       <c r="T137" s="17"/>
       <c r="U137" s="18"/>
     </row>
-    <row r="138" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:21" x14ac:dyDescent="0.25">
       <c r="S138" s="16"/>
       <c r="T138" s="16"/>
       <c r="U138" s="16"/>
     </row>
-    <row r="139" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:21" x14ac:dyDescent="0.25">
       <c r="S139" s="16"/>
       <c r="T139" s="16"/>
       <c r="U139" s="16"/>
     </row>
-    <row r="140" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:21" x14ac:dyDescent="0.25">
       <c r="S140" s="16"/>
       <c r="T140" s="16"/>
       <c r="U140" s="16"/>
@@ -8034,15 +8060,15 @@
       <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.26953125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.453125" customWidth="1"/>
-    <col min="9" max="9" width="14.26953125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.42578125" customWidth="1"/>
+    <col min="9" max="9" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>193</v>
       </c>
@@ -8050,7 +8076,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>252</v>
       </c>
@@ -8061,7 +8087,7 @@
       <c r="J2" s="10"/>
       <c r="K2" s="10"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>253</v>
       </c>
@@ -8072,7 +8098,7 @@
       <c r="J3" s="10"/>
       <c r="K3" s="10"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>254</v>
       </c>
@@ -8083,7 +8109,7 @@
       <c r="J4" s="10"/>
       <c r="K4" s="10"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>255</v>
       </c>
@@ -8094,7 +8120,7 @@
       <c r="J5" s="10"/>
       <c r="K5" s="10"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>256</v>
       </c>
@@ -8105,7 +8131,7 @@
       <c r="D6" s="10"/>
       <c r="K6" s="10"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>39</v>
       </c>
@@ -8114,7 +8140,7 @@
       </c>
       <c r="C7" s="10"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>257</v>
       </c>
@@ -8123,7 +8149,7 @@
       </c>
       <c r="C8" s="10"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>258</v>
       </c>
@@ -8132,7 +8158,7 @@
       </c>
       <c r="C9" s="10"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
         <v>259</v>
       </c>
@@ -8141,7 +8167,7 @@
       </c>
       <c r="C10" s="10"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
         <v>260</v>
       </c>
@@ -8150,7 +8176,7 @@
       </c>
       <c r="C11" s="10"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
         <v>261</v>
       </c>
@@ -8159,7 +8185,7 @@
       </c>
       <c r="C12" s="10"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
         <v>262</v>
       </c>
@@ -8168,7 +8194,7 @@
       </c>
       <c r="C13" s="10"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
         <v>263</v>
       </c>
@@ -8177,7 +8203,7 @@
       </c>
       <c r="C14" s="10"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
         <v>264</v>
       </c>
@@ -8186,7 +8212,7 @@
       </c>
       <c r="C15" s="10"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
         <v>265</v>
       </c>
@@ -8195,7 +8221,7 @@
       </c>
       <c r="C16" s="10"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
         <v>266</v>
       </c>
@@ -8204,7 +8230,7 @@
       </c>
       <c r="C17" s="10"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
         <v>267</v>
       </c>
@@ -8213,7 +8239,7 @@
       </c>
       <c r="C18" s="10"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
         <v>268</v>
       </c>
@@ -8222,7 +8248,7 @@
       </c>
       <c r="C19" s="10"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
         <v>269</v>
       </c>
@@ -8231,7 +8257,7 @@
       </c>
       <c r="C20" s="10"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
         <v>249</v>
       </c>
@@ -8240,7 +8266,7 @@
       </c>
       <c r="C21" s="10"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
         <v>7</v>
       </c>
@@ -8249,7 +8275,7 @@
       </c>
       <c r="C22" s="10"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
         <v>270</v>
       </c>
@@ -8258,7 +8284,7 @@
       </c>
       <c r="C23" s="10"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
         <v>250</v>
       </c>
@@ -8267,7 +8293,7 @@
       </c>
       <c r="C24" s="10"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
         <v>271</v>
       </c>
@@ -8276,7 +8302,7 @@
       </c>
       <c r="C25" s="10"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
         <v>251</v>
       </c>
@@ -8285,7 +8311,7 @@
       </c>
       <c r="C26" s="10"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="9" t="s">
         <v>275</v>
       </c>
@@ -8293,7 +8319,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="9" t="s">
         <v>296</v>
       </c>
@@ -8301,7 +8327,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="9" t="s">
         <v>300</v>
       </c>

</xml_diff>

<commit_message>
Atualizacao de configuracoes 29/04/2025 (+ PSATSALT): arquivo(s) de entrada exemplo(s)
</commit_message>
<xml_diff>
--- a/Configuracao.xlsx
+++ b/Configuracao.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\remocaovies_ECMWF_ENSExtended\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFDC99D0-722C-47D4-B4AF-7350C53B87A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A955CFD9-B8C0-463F-94D4-EFD677BA783E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="945" yWindow="2025" windowWidth="26745" windowHeight="11385" xr2:uid="{49340ABD-EBBA-4697-9F32-382481CBB267}"/>
+    <workbookView xWindow="3750" yWindow="3720" windowWidth="28410" windowHeight="14880" xr2:uid="{49340ABD-EBBA-4697-9F32-382481CBB267}"/>
   </bookViews>
   <sheets>
     <sheet name="Dados" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="304">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="305">
   <si>
     <t>Agua Vermelha</t>
   </si>
@@ -939,13 +939,16 @@
     <t>Apiacas</t>
   </si>
   <si>
-    <t>UHE Canastra</t>
-  </si>
-  <si>
     <t>PSATSALT</t>
   </si>
   <si>
     <t>Cai</t>
+  </si>
+  <si>
+    <t>Salto RS</t>
+  </si>
+  <si>
+    <t>0,46715</t>
   </si>
 </sst>
 </file>
@@ -1427,10 +1430,10 @@
   <dimension ref="A1:U140"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B125" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B116" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="M132" sqref="M132"/>
+      <selection pane="bottomRight" activeCell="Q132" sqref="Q132"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8001,7 +8004,7 @@
     </row>
     <row r="132" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A132" s="3" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="B132" s="5">
         <v>-29.32</v>
@@ -8010,10 +8013,43 @@
         <v>-50.68</v>
       </c>
       <c r="D132" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="E132" s="6">
+        <v>32</v>
+      </c>
+      <c r="F132" s="7">
+        <v>101</v>
+      </c>
+      <c r="G132" s="7">
+        <v>105</v>
+      </c>
+      <c r="H132" s="7">
+        <v>118</v>
+      </c>
+      <c r="I132" s="7">
+        <v>129</v>
+      </c>
+      <c r="J132" s="7">
+        <v>141</v>
+      </c>
+      <c r="K132" s="7">
+        <v>144</v>
+      </c>
+      <c r="L132" t="s">
         <v>302</v>
       </c>
-      <c r="L132" t="s">
-        <v>303</v>
+      <c r="M132" s="7" t="s">
+        <v>304</v>
+      </c>
+      <c r="N132" s="12">
+        <v>0</v>
+      </c>
+      <c r="O132">
+        <v>514</v>
+      </c>
+      <c r="P132">
+        <v>2</v>
       </c>
     </row>
     <row r="135" spans="1:21" x14ac:dyDescent="0.25">

</xml_diff>